<commit_message>
Excel Auswertung Teil 1
</commit_message>
<xml_diff>
--- a/TestDaten/Hand-Joystick-3m.xlsx
+++ b/TestDaten/Hand-Joystick-3m.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Joints7" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Hand.X</t>
   </si>
@@ -43,25 +43,31 @@
     <t>Schulter.Z</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
     <t>Max Abw. [m]</t>
-  </si>
-  <si>
-    <t>Hand</t>
   </si>
   <si>
     <t>Std. Abw [m]</t>
   </si>
   <si>
     <t>Nullpunkt</t>
+  </si>
+  <si>
+    <t>Hand Rechts</t>
+  </si>
+  <si>
+    <t>X [m]</t>
+  </si>
+  <si>
+    <t>Y [m]</t>
+  </si>
+  <si>
+    <t>Z [m]</t>
+  </si>
+  <si>
+    <t>Hüfte</t>
+  </si>
+  <si>
+    <t>Ellb. Rechts</t>
   </si>
 </sst>
 </file>
@@ -386,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -513,39 +519,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -562,16 +539,33 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </bottom>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -626,18 +620,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="6" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -686,6 +679,2842 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-CH"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>X [m]</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Joints7!$A$2:$A$334</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="333"/>
+                <c:pt idx="0">
+                  <c:v>0.25981739999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26124639999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26028820000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26198450000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27010630000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2589591</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26009090000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25666470000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25794339999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2557702</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25460120000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25424409999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26115460000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.25437729999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25424330000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25420029999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25255640000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25220369999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2524459</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.25210929999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.25293450000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25280710000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.26451219999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.25356230000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2610191</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25578109999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.25741049999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.25792969999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.26406429999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.25950640000000003</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.25956420000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.25989430000000002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.26006499999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.2605246</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.26064110000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.26114680000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.2610885</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.26140419999999998</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.26135140000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.26878999999999997</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.26175700000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.26166650000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.26152130000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.26625110000000002</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.2615845</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.26066889999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.26853120000000003</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.26477319999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.26329370000000002</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.26172679999999998</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.26323609999999997</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.26314890000000002</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.26942880000000002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.2634319</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.26294390000000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.26328819999999997</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.2670495</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.26275340000000003</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.26259310000000002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.26103369999999998</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.26587290000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.26011820000000002</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.26732060000000002</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.26038519999999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.2611021</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.27138230000000002</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.26135330000000001</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.26198159999999998</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.2612138</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.261042</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.26136920000000002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.2612273</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.26097120000000001</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.26595289999999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.26527430000000002</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.26160739999999999</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.26157839999999999</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.2469915</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.26104070000000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.26088790000000001</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.26092490000000002</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.2642621</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.26023600000000002</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.2598993</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.25981799999999999</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.26101619999999998</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.25982179999999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.25970799999999999</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.22522590000000001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.22013250000000001</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.22307460000000001</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.2537238</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.28449780000000002</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.28015139999999999</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.2519285</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.25177440000000001</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.25110539999999998</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.25934649999999998</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.25153690000000001</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.26141730000000002</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.25623210000000002</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.25641269999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.25600800000000001</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.25572450000000002</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.25452720000000001</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.25163190000000002</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.25754189999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.25456190000000001</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.25307819999999998</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.25006</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.2480793</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.24797040000000001</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.2500695</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.24955050000000001</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.2496842</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.248803</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.24831729999999999</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.24793680000000001</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.24778839999999999</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.2477423</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.2471121</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.2522471</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.25253219999999998</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.25250860000000003</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.247803</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.2532507</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.25357259999999998</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.24995700000000001</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.24943109999999999</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.249447</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.24867</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.25005159999999998</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.2496855</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.25040839999999998</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.24951400000000001</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.25091229999999998</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.2499149</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.2364272</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.24634780000000001</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.2462675</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.2461438</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.2484875</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.25966159999999999</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.2631944</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.24991260000000001</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.25616800000000001</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.26779629999999999</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.25943090000000002</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.25258819999999998</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.25418499999999999</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.251884</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.25151069999999998</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.25099359999999998</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.25153890000000001</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.25116880000000003</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.23454120000000001</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.23500489999999999</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.22838890000000001</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.22370470000000001</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.2201611</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.21963250000000001</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.25422899999999998</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.2468919</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.24720809999999999</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.25043650000000001</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.2511776</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.25030439999999998</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.25758370000000003</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.25100479999999997</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.25181009999999998</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.25052449999999998</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.24880769999999999</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.2491004</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.248859</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.2491852</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.25025069999999999</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.24860409999999999</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.24845619999999999</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.2491477</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.25793100000000002</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.24956919999999999</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.2494072</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.2496871</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.24885779999999999</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.24755060000000001</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.2476449</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.24799350000000001</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.2506623</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.2469189</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.24635609999999999</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.24655189999999999</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.2485945</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.24574789999999999</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.24812580000000001</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.2476554</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.24490719999999999</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.244945</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.2468205</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.2487531</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.23673849999999999</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.2453717</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.24417430000000001</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.2457464</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.24559</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.24500540000000001</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.24671699999999999</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.2461902</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.25134329999999999</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.24652760000000001</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.2459199</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.24557080000000001</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.24548229999999999</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.2453265</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.24569440000000001</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.2455222</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.24391370000000001</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.2452474</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.24482770000000001</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.24534610000000001</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.24535489999999999</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.2453304</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.24509139999999999</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.24537039999999999</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.24557850000000001</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.24533569999999999</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.24537909999999999</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.2454247</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.24598349999999999</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.24560399999999999</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.24563950000000001</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.24540329999999999</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.24441669999999999</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.2440059</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.24506510000000001</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.2446285</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.24485080000000001</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.25018309999999999</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.2496459</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.24394859999999999</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.24360950000000001</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.24619550000000001</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>0.2406654</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.24101500000000001</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>0.24082120000000001</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.24396519999999999</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.2408622</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>0.23962629999999999</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.24153620000000001</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.24400939999999999</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>0.24484239999999999</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>0.2473487</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>0.2410699</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>0.1809278</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>0.24062710000000001</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>0.23303070000000001</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>0.26627450000000003</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>0.26389410000000002</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>0.24179909999999999</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>0.24201120000000001</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>0.24130299999999999</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>0.24162610000000001</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>0.2418642</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>0.2424655</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>0.24292569999999999</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>0.24305560000000001</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>0.2433873</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>0.24907950000000001</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>0.24015049999999999</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>0.24349860000000001</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>0.24354809999999999</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>0.2423199</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>0.2422298</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>0.2425466</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>0.24268770000000001</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>0.242619</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>0.24390629999999999</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>0.2433903</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>0.24347009999999999</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>0.2430881</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>0.24343909999999999</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>0.2431585</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>0.24340390000000001</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>0.2429414</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>0.2429673</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>0.24300820000000001</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>0.24276600000000001</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>0.24257580000000001</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>0.2430205</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>0.2268994</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>0.2328238</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>0.22678889999999999</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>0.23594899999999999</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>0.243009</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>0.2436972</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>0.24469060000000001</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>0.2137848</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>0.22892000000000001</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>0.2451065</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>0.24498700000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Y [m]</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Joints7!$B$2:$B$334</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="333"/>
+                <c:pt idx="0">
+                  <c:v>-0.15139069999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.15282879999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.1513582</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.15570310000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.12794800000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.15185689999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.15295909999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.14995559999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.15167249999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.1527461</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.15528429999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.15539700000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.12860530000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.1569477</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.15449979999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.15578829999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.15795580000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.15865170000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.1598415</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.16014010000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.15980320000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.16213820000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.15551280000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.1622355</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.1571227</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.16185359999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.16187219999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.161861</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.15861430000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.16113379999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.16130330000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.1611012</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.16121579999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.16224649999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.16168979999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.16203110000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.16210669999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.1622778</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-0.16252269999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.1587527</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-0.16258909999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-0.16280520000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.16246530000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.1607113</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.1600057</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.16031609999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.16611690000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.15913450000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.1592258</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.16137860000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-0.16008559999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-0.15976399999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-0.15605939999999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-0.1600028</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-0.1610482</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-0.1607325</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-0.15929689999999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-0.16171759999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-0.1615009</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-0.1633</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-0.16126470000000001</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-0.1645614</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-0.16184809999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-0.16508719999999999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-0.16265379999999999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-0.15565509999999999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-0.163691</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-0.16355929999999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-0.16428680000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-0.16426940000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-0.16384760000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-0.16434950000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-0.16432620000000001</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-0.16160189999999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-0.16277440000000001</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-0.1654109</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-0.16742280000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-0.1836197</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-0.16724720000000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-0.16697049999999999</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-0.1700093</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-0.17319509999999999</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-0.16822719999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-0.1710343</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-0.1708703</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-0.17294709999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-0.17356369999999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-0.17533309999999999</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-0.1563802</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-0.15121879999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-0.14293719999999999</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-0.1754877</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-0.17327149999999999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-0.17242560000000001</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-0.17746970000000001</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-0.1771558</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-0.17659839999999999</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-0.17519960000000001</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-0.17538290000000001</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-0.17211940000000001</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-0.17242399999999999</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-0.1717563</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-0.17337089999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-0.17319119999999999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-0.17412929999999999</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-0.1763102</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-0.1741887</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-0.1751627</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-0.176986</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-0.1771114</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-0.17683080000000001</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-0.1768593</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>-0.17618519999999999</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-0.17567659999999999</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>-0.1752629</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>-0.174488</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>-0.1752264</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>-0.17479149999999999</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>-0.1746123</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>-0.17534959999999999</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>-0.1757958</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>-0.17236750000000001</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>-0.17223630000000001</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>-0.17217640000000001</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>-0.1758641</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>-0.17201810000000001</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>-0.16973920000000001</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>-0.17230200000000001</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-0.175537</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-0.17547499999999999</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-0.17579239999999999</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>-0.17614189999999999</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>-0.17580889999999999</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>-0.17480780000000001</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>-0.17511979999999999</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>-0.1745891</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>-0.1753991</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>-0.1823747</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>-0.18040249999999999</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>-0.18011060000000001</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>-0.1786692</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>-0.1745208</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>-0.1724194</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>-0.1694985</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>-0.17171159999999999</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>-0.17610310000000001</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>-0.2000063</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>-0.19951920000000001</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>-0.17908830000000001</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>-0.17401949999999999</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>-0.1763496</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>-0.1761673</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>-0.1759222</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>-0.17637649999999999</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>-0.17610129999999999</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>-0.16509370000000001</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>-0.17069889999999999</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>-0.16353400000000001</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>-0.16275870000000001</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>-0.16226019999999999</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>-0.16204189999999999</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>-0.1757793</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>-0.17543249999999999</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>-0.17491110000000001</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>-0.17372199999999999</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>-0.1719002</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>-0.172212</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>-0.20004269999999999</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>-0.17287620000000001</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>-0.17273330000000001</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>-0.1731683</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>-0.17105339999999999</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>-0.1692671</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>-0.16957900000000001</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>-0.16945930000000001</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>-0.1694116</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>-0.1721569</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>-0.17228099999999999</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>-0.16913329999999999</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>-0.1821634</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>-0.17177010000000001</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>-0.17163639999999999</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>-0.17189589999999999</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>-0.17241400000000001</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>-0.1728094</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>-0.17260610000000001</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>-0.17232910000000001</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>-0.17119309999999999</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>-0.1698683</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>-0.1723972</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>-0.171519</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>-0.16201360000000001</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>-0.16683970000000001</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>-0.17155909999999999</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>-0.17177439999999999</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>-0.17097789999999999</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>-0.1738179</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>-0.16960529999999999</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>-0.17406930000000001</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>-0.186278</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>-0.18017820000000001</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>-0.1801295</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>-0.17620469999999999</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>-0.17579439999999999</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>-0.1765998</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>-0.1743722</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>-0.17409359999999999</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>-0.17436840000000001</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>-0.17479159999999999</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>-0.1734465</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>-0.17272789999999999</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>-0.17268649999999999</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>-0.1725795</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>-0.1720132</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>-0.17321130000000001</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>-0.1754877</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>-0.1734407</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>-0.1736674</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>-0.17247090000000001</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>-0.17252239999999999</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>-0.17262669999999999</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>-0.1737042</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>-0.17362259999999999</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>-0.17423669999999999</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>-0.1742715</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>-0.17415259999999999</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>-0.17427309999999999</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>-0.17362349999999999</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>-0.17311550000000001</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>-0.17350489999999999</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>-0.17313239999999999</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>-0.17295840000000001</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>-0.17278679999999999</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>-0.17107249999999999</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>-0.17249990000000001</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>-0.172482</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>-0.17087459999999999</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>-0.17098720000000001</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>-0.17212669999999999</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>-0.172212</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>-0.18308340000000001</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>-0.17314089999999999</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>-0.17332320000000001</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>-0.1733384</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>-0.1716839</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>-0.1730302</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>-0.17222009999999999</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>-0.1739957</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>-0.1766075</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>-0.17417440000000001</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>-0.16159960000000001</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>-0.1716712</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>-0.18603130000000001</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>-0.17088059999999999</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>-0.20886160000000001</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>-0.14192270000000001</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>-0.1427747</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>-0.17288919999999999</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>-0.17270750000000001</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>-0.1711231</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>-0.17153489999999999</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>-0.1718623</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>-0.17180609999999999</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>-0.17191709999999999</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>-0.17154359999999999</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>-0.17215839999999999</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>-0.12677859999999999</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>-0.1438033</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>-0.17755470000000001</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>-0.17730699999999999</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>-0.17470079999999999</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>-0.1750931</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>-0.17506869999999999</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>-0.1750506</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>-0.1773448</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>-0.17532310000000001</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>-0.17520050000000001</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>-0.1751366</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>-0.1751248</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>-0.17468729999999999</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>-0.17504349999999999</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>-0.17451659999999999</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>-0.1752042</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>-0.1752235</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>-0.1751962</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>-0.17581959999999999</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>-0.1745795</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>-0.17440939999999999</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>-0.16384799999999999</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>-0.1704774</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>-0.16561880000000001</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>-0.20039969999999999</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>-0.17036979999999999</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>-0.1722803</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>-0.17236770000000001</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>-0.18021239999999999</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>-0.18283079999999999</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>-0.17342340000000001</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>-0.17298959999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Z [m]</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Joints7!$C$2:$C$334</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="333"/>
+                <c:pt idx="0">
+                  <c:v>3.3008099999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3005390000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2927339999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2952780000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2144620000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3086799999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2999339999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.316446</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3215170000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.322635</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3233920000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3228589999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.2850630000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.319671</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.308675</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3090470000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.3040660000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.3033800000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.2942469999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.2945009999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.297895</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.3167059999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.278035</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.314343</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.283058</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.304551</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.3100130000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.3115869999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.2824800000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.30463</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.3073169999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3056290000000002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.3054000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3077740000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.3073800000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.3094519999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.3100329999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.3103669999999998</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.3099780000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.28281</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.309768</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.3097249999999998</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.309526</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.2807379999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.3009110000000002</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.299086</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.254308</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.3046160000000002</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.3009729999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.3017029999999998</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.3008440000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.3006319999999998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.2790330000000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.3021530000000001</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.3032849999999998</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.302019</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.2846160000000002</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.302867</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.3028040000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.3164920000000002</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.2887360000000001</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.3092419999999998</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.2809010000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.3094570000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.3118479999999999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.291229</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.3181219999999998</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.305758</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.3034080000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.3033589999999999</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.3039529999999999</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.3033939999999999</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.2974700000000001</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.2821829999999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.2840500000000001</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.2946849999999999</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.2954859999999999</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.2680470000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.2930570000000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.290683</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.2774459999999999</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.284729</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.2648389999999998</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.2751229999999998</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.280078</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.2865150000000001</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3.2880250000000002</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.2941050000000001</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.2487720000000002</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.2569430000000001</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.261558</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.3047840000000002</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.2133949999999998</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.2142140000000001</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.3180369999999999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.3159879999999999</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.3089949999999999</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.2734999999999999</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.3105880000000001</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.2744140000000002</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3.2762159999999998</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3.2763979999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>3.2793679999999998</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3.2804519999999999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>3.2787380000000002</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>3.2984110000000002</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>3.2753809999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>3.2782499999999999</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>3.2798820000000002</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>3.2799649999999998</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>3.2871429999999999</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3.2870529999999998</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>3.2837000000000001</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>3.2841019999999999</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>3.2826659999999999</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>3.2908430000000002</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>3.2886980000000001</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>3.2951380000000001</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>3.296354</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>3.2980330000000002</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>3.290165</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>3.2720020000000001</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>3.2714259999999999</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>3.2709519999999999</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>3.289377</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>3.2714650000000001</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>3.2723450000000001</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>3.285361</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>3.2933539999999999</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>3.2931020000000002</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>3.2914439999999998</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>3.3005469999999999</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>3.3000479999999999</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>3.2941950000000002</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>3.2974899999999998</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>3.2924470000000001</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>3.2953209999999999</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>3.2502650000000002</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>3.2864680000000002</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>3.2865950000000002</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>3.2854969999999999</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>3.3017270000000001</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>3.2019449999999998</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>3.2047949999999998</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>3.2965089999999999</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>3.281037</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>3.229759</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>3.2260049999999998</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>3.2708439999999999</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>3.2792849999999998</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>3.2878609999999999</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>3.2882699999999998</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>3.2888289999999998</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>3.2879510000000001</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>3.287652</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>3.2449309999999998</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>3.2528030000000001</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>3.233781</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>3.2350409999999998</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>3.2318190000000002</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>3.2314029999999998</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>3.2777539999999998</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>3.3049390000000001</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>3.3048329999999999</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>3.2833839999999999</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>3.2841990000000001</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>3.2909350000000002</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>3.239576</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>3.296478</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>3.2892220000000001</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>3.297034</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>3.2865929999999999</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>3.2769469999999998</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>3.277047</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>3.2779430000000001</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>3.279121</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>3.2979370000000001</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>3.2977650000000001</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>3.2806929999999999</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>3.2448229999999998</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>3.275369</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>3.2753489999999998</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>3.2853150000000002</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>3.289307</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>3.2927770000000001</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>3.292872</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>3.294019</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>3.2791640000000002</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>3.275725</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>3.2810169999999999</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>3.2786940000000002</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>3.2609249999999999</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>3.2665459999999999</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>3.2836750000000001</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>3.2852450000000002</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>3.268059</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>3.300306</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>3.2678729999999998</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>3.2935660000000002</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>3.2677939999999999</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>3.2824249999999999</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>3.2899289999999999</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>3.2641800000000001</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>3.2659479999999999</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>3.292405</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>3.293418</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>3.2932640000000002</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>3.2340580000000001</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>3.2892570000000001</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>3.288351</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>3.2883110000000002</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>3.2876280000000002</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>3.2861980000000002</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>3.2868409999999999</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>3.28417</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>3.2941569999999998</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>3.2862269999999998</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>3.2901579999999999</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>3.2885689999999999</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>3.2883550000000001</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>3.288313</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>3.2925870000000002</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>3.2918210000000001</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>3.2936139999999998</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>3.2946309999999999</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>3.2943449999999999</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>3.2943120000000001</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>3.2936079999999999</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>3.289126</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>3.2892440000000001</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>3.2903150000000001</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>3.294041</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>3.2934079999999999</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>3.286267</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>3.2799839999999998</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>3.2825449999999998</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>3.1852079999999998</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>3.186385</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>3.2817609999999999</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>3.2813729999999999</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>3.1878030000000002</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>3.275884</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>3.2757269999999998</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>3.2748789999999999</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>3.1879439999999999</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>3.277031</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>3.2383299999999999</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>3.2753079999999999</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>3.185899</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>3.1849120000000002</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>3.185683</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>3.271547</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>3.2718590000000001</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>3.269139</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>3.2293609999999999</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>3.2673179999999999</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>3.2674259999999999</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>3.270016</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>3.2696130000000001</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>3.27223</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>3.2717860000000001</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>3.271973</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>3.2739739999999999</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>3.275369</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>3.2724389999999999</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>3.2739929999999999</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>3.2618269999999998</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>3.2420599999999999</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>3.2782529999999999</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>3.2778640000000001</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>3.2773759999999998</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>3.2777270000000001</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>3.2741600000000002</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>3.2738830000000001</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>3.282597</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>3.2745280000000001</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>3.2771210000000002</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>3.2770060000000001</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>3.2764790000000001</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>3.2723179999999998</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>3.2721140000000002</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>3.2731669999999999</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>3.273285</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>3.2732169999999998</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>3.2732169999999998</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>3.2778119999999999</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>3.2816670000000001</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>3.2785479999999998</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>3.2261009999999999</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>3.2336710000000002</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>3.2316220000000002</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>3.2524860000000002</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>3.2642890000000002</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>3.2728969999999999</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>3.2852549999999998</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>3.2461220000000002</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>3.242483</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>3.2847209999999998</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>3.2830349999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="83947520"/>
+        <c:axId val="83949056"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="83947520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="83949056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="83949056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="83947520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>666749</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -973,15 +3802,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N335"/>
+  <dimension ref="A1:N300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" customWidth="1"/>
   </cols>
@@ -1015,16 +3845,16 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
       <c r="M1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="N1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -1056,19 +3886,19 @@
         <v>3.6668720000000001</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="L2" s="2">
-        <f>AVERAGE(A$2:A$334)</f>
-        <v>0.24993067957957973</v>
-      </c>
-      <c r="M2" s="3">
-        <f>AVERAGE(B$2:B$334)</f>
-        <v>-0.16985005285285279</v>
-      </c>
-      <c r="N2" s="4">
-        <f>AVERAGE(C$2:C$334)</f>
-        <v>3.2801115435435459</v>
+        <f>AVERAGE(A$2:A$300)</f>
+        <v>0.25045426655518405</v>
+      </c>
+      <c r="M2" s="2">
+        <f t="shared" ref="M2:N2" si="0">AVERAGE(B$2:B$300)</f>
+        <v>-0.16960488428093634</v>
+      </c>
+      <c r="N2" s="5">
+        <f t="shared" si="0"/>
+        <v>3.2812153879598691</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1100,19 +3930,19 @@
         <v>3.6678350000000002</v>
       </c>
       <c r="K3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="5">
-        <f>MAX(ABS(AVERAGE(A$2:A$334)-MAX(A$2:A$334)), ABS(AVERAGE(A$2:A$334)-MIN(A$2:A$334)))</f>
-        <v>6.9002879579579735E-2</v>
-      </c>
-      <c r="M3" s="6">
-        <f>MAX(ABS(AVERAGE(B$2:B$334)-MAX(B$2:B$334)), ABS(AVERAGE(B$2:B$334)-MIN(B$2:B$334)))</f>
-        <v>5.0342052852852787E-2</v>
-      </c>
-      <c r="N3" s="7">
-        <f>MAX(ABS(AVERAGE(C$2:C$334)-MAX(C$2:C$334)), ABS(AVERAGE(C$2:C$334)-MIN(C$2:C$334)))</f>
-        <v>9.5199543543545762E-2</v>
+        <v>9</v>
+      </c>
+      <c r="L3" s="3">
+        <f>MAX(ABS(AVERAGE(A$2:A$300)-MAX(A$2:A$300)), ABS(AVERAGE(A$2:A$300)-MIN(A$2:A$300)))</f>
+        <v>6.9526466555184047E-2</v>
+      </c>
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:N3" si="1">MAX(ABS(AVERAGE(B$2:B$300)-MAX(B$2:B$300)), ABS(AVERAGE(B$2:B$300)-MIN(B$2:B$300)))</f>
+        <v>4.282628428093635E-2</v>
+      </c>
+      <c r="N3" s="6">
+        <f t="shared" si="1"/>
+        <v>9.6303387959868925E-2</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1144,19 +3974,19 @@
         <v>3.6680619999999999</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="8">
-        <f>STDEV(A$2:A$334)</f>
-        <v>1.0263214680857301E-2</v>
-      </c>
-      <c r="M4" s="9">
-        <f>STDEV(B$2:B$334)</f>
-        <v>9.7012799653009695E-3</v>
-      </c>
-      <c r="N4" s="10">
-        <f>STDEV(C$2:C$334)</f>
-        <v>2.6027486880625651E-2</v>
+        <v>10</v>
+      </c>
+      <c r="L4" s="4">
+        <f>STDEV(A$2:A$300)</f>
+        <v>1.0619006100666477E-2</v>
+      </c>
+      <c r="M4" s="4">
+        <f t="shared" ref="M4:N4" si="2">STDEV(B$2:B$300)</f>
+        <v>9.7093441452133222E-3</v>
+      </c>
+      <c r="N4" s="7">
+        <f t="shared" si="2"/>
+        <v>2.5711688242089005E-2</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1216,6 +4046,18 @@
       <c r="I6">
         <v>3.6671900000000002</v>
       </c>
+      <c r="K6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7">
@@ -1245,6 +4087,21 @@
       <c r="I7">
         <v>3.6673840000000002</v>
       </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="2">
+        <f>AVERAGE(D$2:D$300)</f>
+        <v>0.20634333177257519</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" ref="M7:N7" si="3">AVERAGE(E$2:E$300)</f>
+        <v>-0.19207424113712368</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="3"/>
+        <v>3.5797320167224083</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8">
@@ -1274,6 +4131,21 @@
       <c r="I8">
         <v>3.6677170000000001</v>
       </c>
+      <c r="K8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="8">
+        <f>MAX(ABS(AVERAGE(D$2:D$300)-MAX(D$2:D$300)), ABS(AVERAGE(D$2:D$300)-MIN(D$2:D$300)))</f>
+        <v>4.7126168227424825E-2</v>
+      </c>
+      <c r="M8" s="8">
+        <f t="shared" ref="M8:N8" si="4">MAX(ABS(AVERAGE(E$2:E$300)-MAX(E$2:E$300)), ABS(AVERAGE(E$2:E$300)-MIN(E$2:E$300)))</f>
+        <v>4.5687858862876324E-2</v>
+      </c>
+      <c r="N8" s="9">
+        <f t="shared" si="4"/>
+        <v>5.3792016722408409E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9">
@@ -1303,6 +4175,21 @@
       <c r="I9">
         <v>3.6679629999999999</v>
       </c>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="4">
+        <f>STDEV(D$2:D$300)</f>
+        <v>1.3335666577090526E-2</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" ref="M9:N9" si="5">STDEV(E$2:E$300)</f>
+        <v>1.2641688134480951E-2</v>
+      </c>
+      <c r="N9" s="7">
+        <f t="shared" si="5"/>
+        <v>1.3339757487119311E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10">
@@ -1361,6 +4248,18 @@
       <c r="I11">
         <v>3.6677059999999999</v>
       </c>
+      <c r="K11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12">
@@ -1390,6 +4289,21 @@
       <c r="I12">
         <v>3.6677219999999999</v>
       </c>
+      <c r="K12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="2">
+        <f>AVERAGE(G$2:G$300)</f>
+        <v>0.18444071304347817</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" ref="M12:N12" si="6">AVERAGE(H$2:H$300)</f>
+        <v>2.7604605819398012E-2</v>
+      </c>
+      <c r="N12" s="5">
+        <f t="shared" si="6"/>
+        <v>3.6536097591973236</v>
+      </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13">
@@ -1419,6 +4333,21 @@
       <c r="I13">
         <v>3.6671320000000001</v>
       </c>
+      <c r="K13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="3">
+        <f>MAX(ABS(AVERAGE(G$2:G$300)-MAX(G$2:G$300)), ABS(AVERAGE(G$2:G$300)-MIN(G$2:G$300)))</f>
+        <v>2.0008586956521829E-2</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" ref="M13:N13" si="7">MAX(ABS(AVERAGE(H$2:H$300)-MAX(H$2:H$300)), ABS(AVERAGE(H$2:H$300)-MIN(H$2:H$300)))</f>
+        <v>5.063865819398012E-3</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="7"/>
+        <v>1.7552240802676256E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14">
@@ -1448,6 +4377,21 @@
       <c r="I14">
         <v>3.6671680000000002</v>
       </c>
+      <c r="K14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="4">
+        <f>STDEV(G$2:G$300)</f>
+        <v>6.0402493313574026E-3</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" ref="M14:N14" si="8">STDEV(H$2:H$300)</f>
+        <v>2.4947829147377457E-3</v>
+      </c>
+      <c r="N14" s="7">
+        <f t="shared" si="8"/>
+        <v>8.8468797340682647E-3</v>
+      </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15">
@@ -9743,999 +12687,9 @@
         <v>3.644698</v>
       </c>
     </row>
-    <row r="301" spans="1:9">
-      <c r="A301">
-        <v>0.24515100000000001</v>
-      </c>
-      <c r="B301">
-        <v>-0.1729137</v>
-      </c>
-      <c r="C301">
-        <v>3.2841490000000002</v>
-      </c>
-      <c r="D301">
-        <v>0.21508530000000001</v>
-      </c>
-      <c r="E301">
-        <v>-0.18536279999999999</v>
-      </c>
-      <c r="F301">
-        <v>3.6026929999999999</v>
-      </c>
-      <c r="G301">
-        <v>0.177984</v>
-      </c>
-      <c r="H301">
-        <v>2.3180780000000002E-2</v>
-      </c>
-      <c r="I301">
-        <v>3.6447400000000001</v>
-      </c>
-    </row>
-    <row r="302" spans="1:9">
-      <c r="A302">
-        <v>0.2454875</v>
-      </c>
-      <c r="B302">
-        <v>-0.17392940000000001</v>
-      </c>
-      <c r="C302">
-        <v>3.286327</v>
-      </c>
-      <c r="D302">
-        <v>0.21769350000000001</v>
-      </c>
-      <c r="E302">
-        <v>-0.18376390000000001</v>
-      </c>
-      <c r="F302">
-        <v>3.6045419999999999</v>
-      </c>
-      <c r="G302">
-        <v>0.17818790000000001</v>
-      </c>
-      <c r="H302">
-        <v>2.340764E-2</v>
-      </c>
-      <c r="I302">
-        <v>3.6452369999999998</v>
-      </c>
-    </row>
-    <row r="303" spans="1:9">
-      <c r="A303">
-        <v>0.25126710000000002</v>
-      </c>
-      <c r="B303">
-        <v>-0.17408170000000001</v>
-      </c>
-      <c r="C303">
-        <v>3.2128290000000002</v>
-      </c>
-      <c r="D303">
-        <v>0.21941849999999999</v>
-      </c>
-      <c r="E303">
-        <v>-0.1821836</v>
-      </c>
-      <c r="F303">
-        <v>3.603847</v>
-      </c>
-      <c r="G303">
-        <v>0.17823990000000001</v>
-      </c>
-      <c r="H303">
-        <v>2.3337770000000001E-2</v>
-      </c>
-      <c r="I303">
-        <v>3.6453280000000001</v>
-      </c>
-    </row>
-    <row r="304" spans="1:9">
-      <c r="A304">
-        <v>0.2429964</v>
-      </c>
-      <c r="B304">
-        <v>-0.1755652</v>
-      </c>
-      <c r="C304">
-        <v>3.2875749999999999</v>
-      </c>
-      <c r="D304">
-        <v>0.2190783</v>
-      </c>
-      <c r="E304">
-        <v>-0.1821622</v>
-      </c>
-      <c r="F304">
-        <v>3.6036700000000002</v>
-      </c>
-      <c r="G304">
-        <v>0.1783894</v>
-      </c>
-      <c r="H304">
-        <v>2.3401149999999999E-2</v>
-      </c>
-      <c r="I304">
-        <v>3.6455540000000002</v>
-      </c>
-    </row>
-    <row r="305" spans="1:9">
-      <c r="A305">
-        <v>0.24316280000000001</v>
-      </c>
-      <c r="B305">
-        <v>-0.17556530000000001</v>
-      </c>
-      <c r="C305">
-        <v>3.2877320000000001</v>
-      </c>
-      <c r="D305">
-        <v>0.2158032</v>
-      </c>
-      <c r="E305">
-        <v>-0.1823893</v>
-      </c>
-      <c r="F305">
-        <v>3.6014659999999998</v>
-      </c>
-      <c r="G305">
-        <v>0.17872689999999999</v>
-      </c>
-      <c r="H305">
-        <v>2.3635260000000002E-2</v>
-      </c>
-      <c r="I305">
-        <v>3.6457090000000001</v>
-      </c>
-    </row>
-    <row r="306" spans="1:9">
-      <c r="A306">
-        <v>0.2434733</v>
-      </c>
-      <c r="B306">
-        <v>-0.17521990000000001</v>
-      </c>
-      <c r="C306">
-        <v>3.2881360000000002</v>
-      </c>
-      <c r="D306">
-        <v>0.20793880000000001</v>
-      </c>
-      <c r="E306">
-        <v>-0.1935375</v>
-      </c>
-      <c r="F306">
-        <v>3.5911080000000002</v>
-      </c>
-      <c r="G306">
-        <v>0.17914289999999999</v>
-      </c>
-      <c r="H306">
-        <v>2.336827E-2</v>
-      </c>
-      <c r="I306">
-        <v>3.6458840000000001</v>
-      </c>
-    </row>
-    <row r="307" spans="1:9">
-      <c r="A307">
-        <v>0.2439173</v>
-      </c>
-      <c r="B307">
-        <v>-0.1750418</v>
-      </c>
-      <c r="C307">
-        <v>3.283668</v>
-      </c>
-      <c r="D307">
-        <v>0.2072879</v>
-      </c>
-      <c r="E307">
-        <v>-0.19428190000000001</v>
-      </c>
-      <c r="F307">
-        <v>3.590551</v>
-      </c>
-      <c r="G307">
-        <v>0.1784327</v>
-      </c>
-      <c r="H307">
-        <v>2.362819E-2</v>
-      </c>
-      <c r="I307">
-        <v>3.6456240000000002</v>
-      </c>
-    </row>
-    <row r="308" spans="1:9">
-      <c r="A308">
-        <v>0.24362929999999999</v>
-      </c>
-      <c r="B308">
-        <v>-0.17384479999999999</v>
-      </c>
-      <c r="C308">
-        <v>3.287455</v>
-      </c>
-      <c r="D308">
-        <v>0.19736190000000001</v>
-      </c>
-      <c r="E308">
-        <v>-0.19464419999999999</v>
-      </c>
-      <c r="F308">
-        <v>3.5786069999999999</v>
-      </c>
-      <c r="G308">
-        <v>0.17849300000000001</v>
-      </c>
-      <c r="H308">
-        <v>2.3762100000000001E-2</v>
-      </c>
-      <c r="I308">
-        <v>3.6457830000000002</v>
-      </c>
-    </row>
-    <row r="309" spans="1:9">
-      <c r="A309">
-        <v>0.24325820000000001</v>
-      </c>
-      <c r="B309">
-        <v>-0.1740786</v>
-      </c>
-      <c r="C309">
-        <v>3.2877860000000001</v>
-      </c>
-      <c r="D309">
-        <v>0.19699169999999999</v>
-      </c>
-      <c r="E309">
-        <v>-0.19485130000000001</v>
-      </c>
-      <c r="F309">
-        <v>3.5780650000000001</v>
-      </c>
-      <c r="G309">
-        <v>0.17862800000000001</v>
-      </c>
-      <c r="H309">
-        <v>2.4031159999999999E-2</v>
-      </c>
-      <c r="I309">
-        <v>3.6457440000000001</v>
-      </c>
-    </row>
-    <row r="310" spans="1:9">
-      <c r="A310">
-        <v>0.24357229999999999</v>
-      </c>
-      <c r="B310">
-        <v>-0.17403940000000001</v>
-      </c>
-      <c r="C310">
-        <v>3.2841279999999999</v>
-      </c>
-      <c r="D310">
-        <v>0.1972111</v>
-      </c>
-      <c r="E310">
-        <v>-0.1952199</v>
-      </c>
-      <c r="F310">
-        <v>3.5783520000000002</v>
-      </c>
-      <c r="G310">
-        <v>0.17829780000000001</v>
-      </c>
-      <c r="H310">
-        <v>2.4013380000000001E-2</v>
-      </c>
-      <c r="I310">
-        <v>3.6458020000000002</v>
-      </c>
-    </row>
-    <row r="311" spans="1:9">
-      <c r="A311">
-        <v>0.24386550000000001</v>
-      </c>
-      <c r="B311">
-        <v>-0.17364379999999999</v>
-      </c>
-      <c r="C311">
-        <v>3.2818160000000001</v>
-      </c>
-      <c r="D311">
-        <v>0.19739780000000001</v>
-      </c>
-      <c r="E311">
-        <v>-0.19559509999999999</v>
-      </c>
-      <c r="F311">
-        <v>3.5783100000000001</v>
-      </c>
-      <c r="G311">
-        <v>0.17805599999999999</v>
-      </c>
-      <c r="H311">
-        <v>2.3945580000000001E-2</v>
-      </c>
-      <c r="I311">
-        <v>3.645702</v>
-      </c>
-    </row>
-    <row r="312" spans="1:9">
-      <c r="A312">
-        <v>0.2443765</v>
-      </c>
-      <c r="B312">
-        <v>-0.1723605</v>
-      </c>
-      <c r="C312">
-        <v>3.2803309999999999</v>
-      </c>
-      <c r="D312">
-        <v>0.2160975</v>
-      </c>
-      <c r="E312">
-        <v>-0.19326080000000001</v>
-      </c>
-      <c r="F312">
-        <v>3.6219619999999999</v>
-      </c>
-      <c r="G312">
-        <v>0.17811460000000001</v>
-      </c>
-      <c r="H312">
-        <v>2.3668620000000001E-2</v>
-      </c>
-      <c r="I312">
-        <v>3.6458780000000002</v>
-      </c>
-    </row>
-    <row r="313" spans="1:9">
-      <c r="A313">
-        <v>0.2443601</v>
-      </c>
-      <c r="B313">
-        <v>-0.1723239</v>
-      </c>
-      <c r="C313">
-        <v>3.2803800000000001</v>
-      </c>
-      <c r="D313">
-        <v>0.21450849999999999</v>
-      </c>
-      <c r="E313">
-        <v>-0.19315209999999999</v>
-      </c>
-      <c r="F313">
-        <v>3.620152</v>
-      </c>
-      <c r="G313">
-        <v>0.1781838</v>
-      </c>
-      <c r="H313">
-        <v>2.3485789999999999E-2</v>
-      </c>
-      <c r="I313">
-        <v>3.6458970000000002</v>
-      </c>
-    </row>
-    <row r="314" spans="1:9">
-      <c r="A314">
-        <v>0.24407570000000001</v>
-      </c>
-      <c r="B314">
-        <v>-0.17272000000000001</v>
-      </c>
-      <c r="C314">
-        <v>3.2869929999999998</v>
-      </c>
-      <c r="D314">
-        <v>0.20817649999999999</v>
-      </c>
-      <c r="E314">
-        <v>-0.1935461</v>
-      </c>
-      <c r="F314">
-        <v>3.6144020000000001</v>
-      </c>
-      <c r="G314">
-        <v>0.17799329999999999</v>
-      </c>
-      <c r="H314">
-        <v>2.356668E-2</v>
-      </c>
-      <c r="I314">
-        <v>3.6456870000000001</v>
-      </c>
-    </row>
-    <row r="315" spans="1:9">
-      <c r="A315">
-        <v>0.2436516</v>
-      </c>
-      <c r="B315">
-        <v>-0.17343049999999999</v>
-      </c>
-      <c r="C315">
-        <v>3.2868810000000002</v>
-      </c>
-      <c r="D315">
-        <v>0.2084027</v>
-      </c>
-      <c r="E315">
-        <v>-0.1982101</v>
-      </c>
-      <c r="F315">
-        <v>3.6041500000000002</v>
-      </c>
-      <c r="G315">
-        <v>0.17796809999999999</v>
-      </c>
-      <c r="H315">
-        <v>2.362436E-2</v>
-      </c>
-      <c r="I315">
-        <v>3.6453920000000002</v>
-      </c>
-    </row>
-    <row r="316" spans="1:9">
-      <c r="A316">
-        <v>0.2447927</v>
-      </c>
-      <c r="B316">
-        <v>-0.1749262</v>
-      </c>
-      <c r="C316">
-        <v>3.2914029999999999</v>
-      </c>
-      <c r="D316">
-        <v>0.21089089999999999</v>
-      </c>
-      <c r="E316">
-        <v>-0.19872590000000001</v>
-      </c>
-      <c r="F316">
-        <v>3.5993140000000001</v>
-      </c>
-      <c r="G316">
-        <v>0.17953810000000001</v>
-      </c>
-      <c r="H316">
-        <v>2.3785830000000001E-2</v>
-      </c>
-      <c r="I316">
-        <v>3.6460300000000001</v>
-      </c>
-    </row>
-    <row r="317" spans="1:9">
-      <c r="A317">
-        <v>0.24445610000000001</v>
-      </c>
-      <c r="B317">
-        <v>-0.17524410000000001</v>
-      </c>
-      <c r="C317">
-        <v>3.2834319999999999</v>
-      </c>
-      <c r="D317">
-        <v>0.21373600000000001</v>
-      </c>
-      <c r="E317">
-        <v>-0.19279370000000001</v>
-      </c>
-      <c r="F317">
-        <v>3.6014949999999999</v>
-      </c>
-      <c r="G317">
-        <v>0.17947279999999999</v>
-      </c>
-      <c r="H317">
-        <v>2.378429E-2</v>
-      </c>
-      <c r="I317">
-        <v>3.6460119999999998</v>
-      </c>
-    </row>
-    <row r="318" spans="1:9">
-      <c r="A318">
-        <v>0.25161109999999998</v>
-      </c>
-      <c r="B318">
-        <v>-0.17407690000000001</v>
-      </c>
-      <c r="C318">
-        <v>3.2157680000000002</v>
-      </c>
-      <c r="D318">
-        <v>0.2194989</v>
-      </c>
-      <c r="E318">
-        <v>-0.18981000000000001</v>
-      </c>
-      <c r="F318">
-        <v>3.6060469999999998</v>
-      </c>
-      <c r="G318">
-        <v>0.1794589</v>
-      </c>
-      <c r="H318">
-        <v>2.37576E-2</v>
-      </c>
-      <c r="I318">
-        <v>3.6460599999999999</v>
-      </c>
-    </row>
-    <row r="319" spans="1:9">
-      <c r="A319">
-        <v>0.2442802</v>
-      </c>
-      <c r="B319">
-        <v>-0.173905</v>
-      </c>
-      <c r="C319">
-        <v>3.2861030000000002</v>
-      </c>
-      <c r="D319">
-        <v>0.2195684</v>
-      </c>
-      <c r="E319">
-        <v>-0.18949260000000001</v>
-      </c>
-      <c r="F319">
-        <v>3.6060140000000001</v>
-      </c>
-      <c r="G319">
-        <v>0.17915429999999999</v>
-      </c>
-      <c r="H319">
-        <v>2.3907709999999999E-2</v>
-      </c>
-      <c r="I319">
-        <v>3.645715</v>
-      </c>
-    </row>
-    <row r="320" spans="1:9">
-      <c r="A320">
-        <v>0.2421381</v>
-      </c>
-      <c r="B320">
-        <v>-0.17389569999999999</v>
-      </c>
-      <c r="C320">
-        <v>3.274467</v>
-      </c>
-      <c r="D320">
-        <v>0.21933610000000001</v>
-      </c>
-      <c r="E320">
-        <v>-0.1887615</v>
-      </c>
-      <c r="F320">
-        <v>3.6049799999999999</v>
-      </c>
-      <c r="G320">
-        <v>0.1791364</v>
-      </c>
-      <c r="H320">
-        <v>2.3967769999999999E-2</v>
-      </c>
-      <c r="I320">
-        <v>3.645705</v>
-      </c>
-    </row>
-    <row r="321" spans="1:9">
-      <c r="A321">
-        <v>0.24209430000000001</v>
-      </c>
-      <c r="B321">
-        <v>-0.17375740000000001</v>
-      </c>
-      <c r="C321">
-        <v>3.2748110000000001</v>
-      </c>
-      <c r="D321">
-        <v>0.2206592</v>
-      </c>
-      <c r="E321">
-        <v>-0.1873927</v>
-      </c>
-      <c r="F321">
-        <v>3.606795</v>
-      </c>
-      <c r="G321">
-        <v>0.1792706</v>
-      </c>
-      <c r="H321">
-        <v>2.4004629999999999E-2</v>
-      </c>
-      <c r="I321">
-        <v>3.6458339999999998</v>
-      </c>
-    </row>
-    <row r="322" spans="1:9">
-      <c r="A322">
-        <v>0.24131089999999999</v>
-      </c>
-      <c r="B322">
-        <v>-0.1758892</v>
-      </c>
-      <c r="C322">
-        <v>3.2156799999999999</v>
-      </c>
-      <c r="D322">
-        <v>0.22074849999999999</v>
-      </c>
-      <c r="E322">
-        <v>-0.1860048</v>
-      </c>
-      <c r="F322">
-        <v>3.6068159999999998</v>
-      </c>
-      <c r="G322">
-        <v>0.1788564</v>
-      </c>
-      <c r="H322">
-        <v>2.3852450000000001E-2</v>
-      </c>
-      <c r="I322">
-        <v>3.6454939999999998</v>
-      </c>
-    </row>
-    <row r="323" spans="1:9">
-      <c r="A323">
-        <v>0.24339440000000001</v>
-      </c>
-      <c r="B323">
-        <v>-0.17277110000000001</v>
-      </c>
-      <c r="C323">
-        <v>3.2165279999999998</v>
-      </c>
-      <c r="D323">
-        <v>0.22119620000000001</v>
-      </c>
-      <c r="E323">
-        <v>-0.18581449999999999</v>
-      </c>
-      <c r="F323">
-        <v>3.6074389999999998</v>
-      </c>
-      <c r="G323">
-        <v>0.1785069</v>
-      </c>
-      <c r="H323">
-        <v>2.4115279999999999E-2</v>
-      </c>
-      <c r="I323">
-        <v>3.6451799999999999</v>
-      </c>
-    </row>
-    <row r="324" spans="1:9">
-      <c r="A324">
-        <v>0.2466546</v>
-      </c>
-      <c r="B324">
-        <v>-0.17233090000000001</v>
-      </c>
-      <c r="C324">
-        <v>3.2806820000000001</v>
-      </c>
-      <c r="D324">
-        <v>0.21781980000000001</v>
-      </c>
-      <c r="E324">
-        <v>-0.18522549999999999</v>
-      </c>
-      <c r="F324">
-        <v>3.6047210000000001</v>
-      </c>
-      <c r="G324">
-        <v>0.17826349999999999</v>
-      </c>
-      <c r="H324">
-        <v>2.4083199999999999E-2</v>
-      </c>
-      <c r="I324">
-        <v>3.6451470000000001</v>
-      </c>
-    </row>
-    <row r="325" spans="1:9">
-      <c r="A325">
-        <v>0.24409829999999999</v>
-      </c>
-      <c r="B325">
-        <v>-0.17292080000000001</v>
-      </c>
-      <c r="C325">
-        <v>3.214127</v>
-      </c>
-      <c r="D325">
-        <v>0.21859410000000001</v>
-      </c>
-      <c r="E325">
-        <v>-0.18459310000000001</v>
-      </c>
-      <c r="F325">
-        <v>3.6047750000000001</v>
-      </c>
-      <c r="G325">
-        <v>0.178232</v>
-      </c>
-      <c r="H325">
-        <v>2.484828E-2</v>
-      </c>
-      <c r="I325">
-        <v>3.6454629999999999</v>
-      </c>
-    </row>
-    <row r="326" spans="1:9">
-      <c r="A326">
-        <v>0.2464055</v>
-      </c>
-      <c r="B326">
-        <v>-0.1718962</v>
-      </c>
-      <c r="C326">
-        <v>3.280567</v>
-      </c>
-      <c r="D326">
-        <v>0.20906240000000001</v>
-      </c>
-      <c r="E326">
-        <v>-0.1834895</v>
-      </c>
-      <c r="F326">
-        <v>3.5725850000000001</v>
-      </c>
-      <c r="G326">
-        <v>0.1776375</v>
-      </c>
-      <c r="H326">
-        <v>2.4251490000000001E-2</v>
-      </c>
-      <c r="I326">
-        <v>3.6447660000000002</v>
-      </c>
-    </row>
-    <row r="327" spans="1:9">
-      <c r="A327">
-        <v>0.26531539999999998</v>
-      </c>
-      <c r="B327">
-        <v>-0.119508</v>
-      </c>
-      <c r="C327">
-        <v>3.2639969999999998</v>
-      </c>
-      <c r="D327">
-        <v>0.2008943</v>
-      </c>
-      <c r="E327">
-        <v>-0.20076469999999999</v>
-      </c>
-      <c r="F327">
-        <v>3.5671210000000002</v>
-      </c>
-      <c r="G327">
-        <v>0.1773972</v>
-      </c>
-      <c r="H327">
-        <v>2.455506E-2</v>
-      </c>
-      <c r="I327">
-        <v>3.6449889999999998</v>
-      </c>
-    </row>
-    <row r="328" spans="1:9">
-      <c r="A328">
-        <v>0.2460116</v>
-      </c>
-      <c r="B328">
-        <v>-0.17012179999999999</v>
-      </c>
-      <c r="C328">
-        <v>3.2818200000000002</v>
-      </c>
-      <c r="D328">
-        <v>0.2050553</v>
-      </c>
-      <c r="E328">
-        <v>-0.18844150000000001</v>
-      </c>
-      <c r="F328">
-        <v>3.5703429999999998</v>
-      </c>
-      <c r="G328">
-        <v>0.1770822</v>
-      </c>
-      <c r="H328">
-        <v>2.463949E-2</v>
-      </c>
-      <c r="I328">
-        <v>3.6450079999999998</v>
-      </c>
-    </row>
-    <row r="329" spans="1:9">
-      <c r="A329">
-        <v>0.2456237</v>
-      </c>
-      <c r="B329">
-        <v>-0.17105129999999999</v>
-      </c>
-      <c r="C329">
-        <v>3.2803960000000001</v>
-      </c>
-      <c r="D329">
-        <v>0.21038309999999999</v>
-      </c>
-      <c r="E329">
-        <v>-0.18315770000000001</v>
-      </c>
-      <c r="F329">
-        <v>3.5793170000000001</v>
-      </c>
-      <c r="G329">
-        <v>0.1773952</v>
-      </c>
-      <c r="H329">
-        <v>2.4499900000000002E-2</v>
-      </c>
-      <c r="I329">
-        <v>3.6448269999999998</v>
-      </c>
-    </row>
-    <row r="330" spans="1:9">
-      <c r="A330">
-        <v>0.2456025</v>
-      </c>
-      <c r="B330">
-        <v>-0.17104430000000001</v>
-      </c>
-      <c r="C330">
-        <v>3.2803300000000002</v>
-      </c>
-      <c r="D330">
-        <v>0.22220699999999999</v>
-      </c>
-      <c r="E330">
-        <v>-0.1788642</v>
-      </c>
-      <c r="F330">
-        <v>3.598967</v>
-      </c>
-      <c r="G330">
-        <v>0.17746419999999999</v>
-      </c>
-      <c r="H330">
-        <v>2.482724E-2</v>
-      </c>
-      <c r="I330">
-        <v>3.64642</v>
-      </c>
-    </row>
-    <row r="331" spans="1:9">
-      <c r="A331">
-        <v>0.2477549</v>
-      </c>
-      <c r="B331">
-        <v>-0.18168999999999999</v>
-      </c>
-      <c r="C331">
-        <v>3.2069450000000002</v>
-      </c>
-      <c r="D331">
-        <v>0.221774</v>
-      </c>
-      <c r="E331">
-        <v>-0.1791275</v>
-      </c>
-      <c r="F331">
-        <v>3.5974650000000001</v>
-      </c>
-      <c r="G331">
-        <v>0.17679890000000001</v>
-      </c>
-      <c r="H331">
-        <v>2.4428729999999999E-2</v>
-      </c>
-      <c r="I331">
-        <v>3.645349</v>
-      </c>
-    </row>
-    <row r="332" spans="1:9">
-      <c r="A332">
-        <v>0.24441470000000001</v>
-      </c>
-      <c r="B332">
-        <v>-0.17131060000000001</v>
-      </c>
-      <c r="C332">
-        <v>3.2805110000000002</v>
-      </c>
-      <c r="D332">
-        <v>0.21951590000000001</v>
-      </c>
-      <c r="E332">
-        <v>-0.17838909999999999</v>
-      </c>
-      <c r="F332">
-        <v>3.5962890000000001</v>
-      </c>
-      <c r="G332">
-        <v>0.17798890000000001</v>
-      </c>
-      <c r="H332">
-        <v>2.5616659999999999E-2</v>
-      </c>
-      <c r="I332">
-        <v>3.6464539999999999</v>
-      </c>
-    </row>
-    <row r="333" spans="1:9">
-      <c r="A333">
-        <v>0.24444060000000001</v>
-      </c>
-      <c r="B333">
-        <v>-0.17157030000000001</v>
-      </c>
-      <c r="C333">
-        <v>3.2800729999999998</v>
-      </c>
-      <c r="D333">
-        <v>0.21974260000000001</v>
-      </c>
-      <c r="E333">
-        <v>-0.1782782</v>
-      </c>
-      <c r="F333">
-        <v>3.5957629999999998</v>
-      </c>
-      <c r="G333">
-        <v>0.17825179999999999</v>
-      </c>
-      <c r="H333">
-        <v>2.5631629999999999E-2</v>
-      </c>
-      <c r="I333">
-        <v>3.6465290000000001</v>
-      </c>
-    </row>
-    <row r="334" spans="1:9">
-      <c r="A334">
-        <v>0.24444640000000001</v>
-      </c>
-      <c r="B334">
-        <v>-0.17153889999999999</v>
-      </c>
-      <c r="C334">
-        <v>3.2799170000000002</v>
-      </c>
-      <c r="D334">
-        <v>0.22033459999999999</v>
-      </c>
-      <c r="E334">
-        <v>-0.2020535</v>
-      </c>
-      <c r="F334">
-        <v>3.6002149999999999</v>
-      </c>
-      <c r="G334">
-        <v>0.17850279999999999</v>
-      </c>
-      <c r="H334">
-        <v>2.5443150000000001E-2</v>
-      </c>
-      <c r="I334">
-        <v>3.6465230000000002</v>
-      </c>
-    </row>
-    <row r="335" spans="1:9">
-      <c r="A335">
-        <v>0.2436161</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>